<commit_message>
gain setup for pga now in setup so does not effect infinite loop
</commit_message>
<xml_diff>
--- a/FYP Finances.xlsx
+++ b/FYP Finances.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>Order Code</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t>Total Spent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">759-0862  </t>
+  </si>
+  <si>
+    <t>AD605ANZ, Dual Voltage Controlled Amplifier Single Ended 4.5 &amp;#8594; 5.5 V 16-Pin PDIP</t>
   </si>
 </sst>
 </file>
@@ -601,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -655,12 +661,12 @@
         <v>1</v>
       </c>
       <c r="F2" s="1">
-        <f>IF(NOT(ISBLANK($D2)),$D2*$E2,"")</f>
+        <f t="shared" ref="F2:F21" si="0">IF(NOT(ISBLANK($D2)),$D2*$E2,"")</f>
         <v>3.45</v>
       </c>
       <c r="G2" s="5">
         <f>SUM(F:F)</f>
-        <v>51.069999999999993</v>
+        <v>63.959999999999994</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -680,7 +686,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1">
-        <f>IF(NOT(ISBLANK($D3)),$D3*$E3,"")</f>
+        <f t="shared" si="0"/>
         <v>1.86</v>
       </c>
       <c r="G3" s="1"/>
@@ -702,7 +708,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="1">
-        <f>IF(NOT(ISBLANK($D4)),$D4*$E4,"")</f>
+        <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
     </row>
@@ -723,7 +729,7 @@
         <v>10</v>
       </c>
       <c r="F5" s="1">
-        <f>IF(NOT(ISBLANK($D5)),$D5*$E5,"")</f>
+        <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
@@ -744,7 +750,7 @@
         <v>5</v>
       </c>
       <c r="F6" s="1">
-        <f>IF(NOT(ISBLANK($D6)),$D6*$E6,"")</f>
+        <f t="shared" si="0"/>
         <v>10.43</v>
       </c>
     </row>
@@ -765,7 +771,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="1">
-        <f>IF(NOT(ISBLANK($D7)),$D7*$E7,"")</f>
+        <f t="shared" si="0"/>
         <v>5.4</v>
       </c>
     </row>
@@ -786,7 +792,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="1">
-        <f>IF(NOT(ISBLANK($D8)),$D8*$E8,"")</f>
+        <f t="shared" si="0"/>
         <v>5.6000000000000005</v>
       </c>
     </row>
@@ -807,7 +813,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="1">
-        <f>IF(NOT(ISBLANK($D9)),$D9*$E9,"")</f>
+        <f t="shared" si="0"/>
         <v>8.51</v>
       </c>
     </row>
@@ -828,7 +834,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="1">
-        <f>IF(NOT(ISBLANK($D10)),$D10*$E10,"")</f>
+        <f t="shared" si="0"/>
         <v>2.62</v>
       </c>
     </row>
@@ -849,7 +855,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="1">
-        <f>IF(NOT(ISBLANK($D11)),$D11*$E11,"")</f>
+        <f t="shared" si="0"/>
         <v>2.54</v>
       </c>
     </row>
@@ -870,7 +876,7 @@
         <v>2</v>
       </c>
       <c r="F12" s="1">
-        <f>IF(NOT(ISBLANK($D12)),$D12*$E12,"")</f>
+        <f t="shared" si="0"/>
         <v>5.4</v>
       </c>
     </row>
@@ -891,7 +897,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="1">
-        <f>IF(NOT(ISBLANK($D13)),$D13*$E13,"")</f>
+        <f t="shared" si="0"/>
         <v>1.95</v>
       </c>
     </row>
@@ -912,7 +918,7 @@
         <v>2</v>
       </c>
       <c r="F14" s="1">
-        <f>IF(NOT(ISBLANK($D14)),$D14*$E14,"")</f>
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
     </row>
@@ -933,25 +939,58 @@
         <v>1</v>
       </c>
       <c r="F15" s="1">
-        <f>IF(NOT(ISBLANK($D15)),$D15*$E15,"")</f>
+        <f t="shared" si="0"/>
         <v>0.71</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="F16" s="1" t="str">
-        <f>IF(NOT(ISBLANK($D16)),$D16*$E16,"")</f>
-        <v/>
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="1">
+        <v>12.89</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <f t="shared" si="0"/>
+        <v>12.89</v>
       </c>
     </row>
     <row r="17" spans="6:6">
       <c r="F17" s="1" t="str">
-        <f>IF(NOT(ISBLANK($D17)),$D17*$E17,"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="18" spans="6:6">
       <c r="F18" s="1" t="str">
-        <f>IF(NOT(ISBLANK($D18)),$D18*$E18,"")</f>
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="6:6">
+      <c r="F19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="6:6">
+      <c r="F20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="6:6">
+      <c r="F21" s="1" t="str">
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -959,6 +998,9 @@
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <ignoredErrors>
+    <ignoredError sqref="F21 F17" emptyCellReference="1"/>
+  </ignoredErrors>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
changed arduino code to account for connections on new pcb
</commit_message>
<xml_diff>
--- a/FYP Finances.xlsx
+++ b/FYP Finances.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="55">
   <si>
     <t>Order Code</t>
   </si>
@@ -161,6 +161,63 @@
   </si>
   <si>
     <t>AD605ANZ, Dual Voltage Controlled Amplifier Single Ended 4.5 &amp;#8594; 5.5 V 16-Pin PDIP</t>
+  </si>
+  <si>
+    <t>Maplin</t>
+  </si>
+  <si>
+    <t>Maplin 4 Pole 3.5mm Stereo Jack Cable 0.75m</t>
+  </si>
+  <si>
+    <t>A61NW</t>
+  </si>
+  <si>
+    <t>HARWIN D01-99 Series, 2.54mm Pitch 20 Way 1 Row Straight PCB Header, Solder Termination, 1.5A</t>
+  </si>
+  <si>
+    <t>547-3302</t>
+  </si>
+  <si>
+    <t>AD605BRZ, Dual Voltage Controlled Amplifier Single Ended 4.5 → 5.5 V 16-Pin SOIC</t>
+  </si>
+  <si>
+    <t>758-9705</t>
+  </si>
+  <si>
+    <t>LUMBERG  1503 13 VP3  SOCKET, 3.5MM JACK, SMT, 4WAY</t>
+  </si>
+  <si>
+    <t>VISHAY BEYSCHLAG  MMA02040E1001BB100  RES, MELF, 1K, 0.1%, 250MW, SMD</t>
+  </si>
+  <si>
+    <t>VISHAY BEYSCHLAG  MMA02040C2201FB300  RES, MELF, 2K2, 1%, 250MW, SMD</t>
+  </si>
+  <si>
+    <t>VISHAY BEYSCHLAG  MMA02040E1002BB100  RESISTOR, 0204 10K</t>
+  </si>
+  <si>
+    <t>3086185RL</t>
+  </si>
+  <si>
+    <t>VISHAY BEYSCHLAG  MMA02040C6802FB300  RES, MELF, 68K, 1%, 250MW, SMD</t>
+  </si>
+  <si>
+    <t>VISHAY BEYSCHLAG  MMA02040E8202BB100  RESISTOR, 0204 82K</t>
+  </si>
+  <si>
+    <t>3086409RL</t>
+  </si>
+  <si>
+    <t>TDK  C3216X7R1C106K160AC  CAP, MLCC, X7R, 10UF, 16V, 1206</t>
+  </si>
+  <si>
+    <t>1907353RL</t>
+  </si>
+  <si>
+    <t>TDK  C3216C0G2J101J060AA  CERAMIC CAPACITOR 100PF 630V, C0G, 5%, 1206</t>
+  </si>
+  <si>
+    <t>PAID MYSELF</t>
   </si>
 </sst>
 </file>
@@ -222,7 +279,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -241,6 +298,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -251,14 +314,120 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -272,12 +441,119 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="111">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -607,10 +883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -619,6 +895,7 @@
     <col min="3" max="3" width="97.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="1"/>
     <col min="6" max="6" width="10.83203125" style="1"/>
+    <col min="7" max="7" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1">
@@ -661,12 +938,12 @@
         <v>1</v>
       </c>
       <c r="F2" s="1">
-        <f t="shared" ref="F2:F21" si="0">IF(NOT(ISBLANK($D2)),$D2*$E2,"")</f>
+        <f t="shared" ref="F2:F30" si="0">IF(NOT(ISBLANK($D2)),$D2*$E2,"")</f>
         <v>3.45</v>
       </c>
       <c r="G2" s="5">
         <f>SUM(F:F)</f>
-        <v>63.959999999999994</v>
+        <v>261.15099999999995</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -964,34 +1241,286 @@
         <v>12.89</v>
       </c>
     </row>
-    <row r="17" spans="6:6">
+    <row r="17" spans="1:7">
       <c r="F17" s="1" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="18" spans="6:6">
-      <c r="F18" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="6:6">
-      <c r="F19" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="6:6">
-      <c r="F20" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="6:6">
-      <c r="F21" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="1">
+        <v>11.99</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18" s="1">
+        <f t="shared" si="0"/>
+        <v>35.97</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="1">
+        <v>13.79</v>
+      </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19" s="1">
+        <f t="shared" si="0"/>
+        <v>68.949999999999989</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1502746</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="E20">
+        <v>5</v>
+      </c>
+      <c r="F20" s="1">
+        <f t="shared" si="0"/>
+        <v>5.6000000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="1">
+        <v>13.91</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21" s="1">
+        <f t="shared" si="0"/>
+        <v>69.55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1368640</v>
+      </c>
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="E22">
+        <v>5</v>
+      </c>
+      <c r="F22" s="1">
+        <f t="shared" si="0"/>
+        <v>2.8050000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="2">
+        <v>3085946</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.214</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
+      </c>
+      <c r="F23" s="1">
+        <f t="shared" si="0"/>
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>3087827</v>
+      </c>
+      <c r="C24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1.5699999999999999E-2</v>
+      </c>
+      <c r="E24">
+        <v>10</v>
+      </c>
+      <c r="F24" s="1">
+        <f t="shared" si="0"/>
+        <v>0.15699999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="E25">
+        <v>10</v>
+      </c>
+      <c r="F25" s="1">
+        <f t="shared" si="0"/>
+        <v>2.09</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="2">
+        <v>3088005</v>
+      </c>
+      <c r="C26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1.78E-2</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26" s="1">
+        <f t="shared" si="0"/>
+        <v>8.8999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="E27">
+        <v>5</v>
+      </c>
+      <c r="F27" s="1">
+        <f t="shared" si="0"/>
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="1">
+        <v>3.6400000000000002E-2</v>
+      </c>
+      <c r="E28">
+        <v>25</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" si="0"/>
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1844418</v>
+      </c>
+      <c r="C29" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="E29">
+        <v>10</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="2">
+        <v>9599568</v>
+      </c>
+      <c r="C30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="1">
+        <v>8.51</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="0"/>
+        <v>8.51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made new project to develop prototype for presentation. will be able to connect to 3 finger boards from the one arduino
</commit_message>
<xml_diff>
--- a/FYP Finances.xlsx
+++ b/FYP Finances.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
   <si>
     <t>Order Code</t>
   </si>
@@ -314,8 +314,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="121">
+  <cellStyleXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -453,7 +475,7 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="121">
+  <cellStyles count="143">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -514,6 +536,17 @@
     <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -574,6 +607,17 @@
     <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -903,10 +947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -958,12 +1002,12 @@
         <v>1</v>
       </c>
       <c r="F2" s="1">
-        <f t="shared" ref="F2:F32" si="0">IF(NOT(ISBLANK($D2)),$D2*$E2,"")</f>
+        <f t="shared" ref="F2:F19" si="0">IF(NOT(ISBLANK($D2)),$D2*$E2,"")</f>
         <v>3.45</v>
       </c>
       <c r="G2" s="5">
         <f>SUM(F:F)</f>
-        <v>263.95599999999996</v>
+        <v>264.32</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1314,44 +1358,44 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="2">
-        <v>1502746</v>
+        <v>21</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="D20" s="1">
-        <v>1.1200000000000001</v>
+        <v>13.91</v>
       </c>
       <c r="E20">
         <v>5</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="0"/>
-        <v>5.6000000000000005</v>
+        <f>IF(NOT(ISBLANK($D20)),$D20*$E20,"")</f>
+        <v>69.55</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>42</v>
+        <v>23</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1368640</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D21" s="1">
-        <v>13.91</v>
+        <v>0.56100000000000005</v>
       </c>
       <c r="E21">
         <v>5</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="0"/>
-        <v>69.55</v>
+        <f>IF(NOT(ISBLANK($D21)),$D21*$E21,"")</f>
+        <v>2.8050000000000002</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1359,20 +1403,20 @@
         <v>23</v>
       </c>
       <c r="B22" s="2">
-        <v>1368640</v>
+        <v>3085946</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D22" s="1">
-        <v>0.56100000000000005</v>
+        <v>0.214</v>
       </c>
       <c r="E22">
         <v>5</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="0"/>
-        <v>2.8050000000000002</v>
+        <f>IF(NOT(ISBLANK($D22)),$D22*$E22,"")</f>
+        <v>1.07</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1380,83 +1424,83 @@
         <v>23</v>
       </c>
       <c r="B23" s="2">
-        <v>3085946</v>
+        <v>3087827</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D23" s="1">
-        <v>0.214</v>
+        <v>1.5699999999999999E-2</v>
       </c>
       <c r="E23">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" si="0"/>
-        <v>1.07</v>
+        <f>IF(NOT(ISBLANK($D23)),$D23*$E23,"")</f>
+        <v>0.15699999999999997</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="2">
-        <v>3087827</v>
+      <c r="B24" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D24" s="1">
-        <v>1.5699999999999999E-2</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="E24">
         <v>10</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="0"/>
-        <v>0.15699999999999997</v>
+        <f>IF(NOT(ISBLANK($D24)),$D24*$E24,"")</f>
+        <v>2.09</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>47</v>
+      <c r="B25" s="2">
+        <v>3088005</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D25" s="1">
-        <v>0.20899999999999999</v>
+        <v>1.78E-2</v>
       </c>
       <c r="E25">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="0"/>
-        <v>2.09</v>
+        <f>IF(NOT(ISBLANK($D25)),$D25*$E25,"")</f>
+        <v>8.8999999999999996E-2</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>23</v>
       </c>
-      <c r="B26" s="2">
-        <v>3088005</v>
+      <c r="B26" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D26" s="1">
-        <v>1.78E-2</v>
+        <v>0.25800000000000001</v>
       </c>
       <c r="E26">
         <v>5</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" si="0"/>
-        <v>8.8999999999999996E-2</v>
+        <f>IF(NOT(ISBLANK($D26)),$D26*$E26,"")</f>
+        <v>1.29</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1464,41 +1508,41 @@
         <v>23</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D27" s="1">
-        <v>0.25800000000000001</v>
+        <v>3.6400000000000002E-2</v>
       </c>
       <c r="E27">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="0"/>
-        <v>1.29</v>
+        <f>IF(NOT(ISBLANK($D27)),$D27*$E27,"")</f>
+        <v>0.91</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>52</v>
+      <c r="B28" s="2">
+        <v>1844418</v>
       </c>
       <c r="C28" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D28" s="1">
-        <v>3.6400000000000002E-2</v>
+        <v>0.02</v>
       </c>
       <c r="E28">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F28" s="1">
-        <f t="shared" si="0"/>
-        <v>0.91</v>
+        <f>IF(NOT(ISBLANK($D28)),$D28*$E28,"")</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1506,41 +1550,41 @@
         <v>23</v>
       </c>
       <c r="B29" s="2">
-        <v>1844418</v>
+        <v>9599568</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="D29" s="1">
-        <v>0.02</v>
+        <v>8.51</v>
       </c>
       <c r="E29">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F29" s="1">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" t="s">
+        <f>IF(NOT(ISBLANK($D29)),$D29*$E29,"")</f>
+        <v>8.51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="2">
-        <v>9599568</v>
-      </c>
-      <c r="C30" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="1">
-        <v>8.51</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-      <c r="F30" s="1">
-        <f t="shared" si="0"/>
-        <v>8.51</v>
+      <c r="B31" s="2">
+        <v>1368640</v>
+      </c>
+      <c r="C31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
+      <c r="F31" s="1">
+        <f>IF(NOT(ISBLANK($D31)),$D31*$E31,"")</f>
+        <v>2.8050000000000002</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1548,20 +1592,41 @@
         <v>23</v>
       </c>
       <c r="B32" s="2">
-        <v>1368640</v>
+        <v>1502746</v>
       </c>
       <c r="C32" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D32" s="1">
-        <v>0.56100000000000005</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="E32">
         <v>5</v>
       </c>
       <c r="F32" s="1">
-        <f t="shared" si="0"/>
-        <v>2.8050000000000002</v>
+        <f>IF(NOT(ISBLANK($D32)),$D32*$E32,"")</f>
+        <v>5.6000000000000005</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="1">
+        <v>3.6400000000000002E-2</v>
+      </c>
+      <c r="E33">
+        <v>10</v>
+      </c>
+      <c r="F33" s="1">
+        <f>IF(NOT(ISBLANK($D33)),$D33*$E33,"")</f>
+        <v>0.36399999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1569,7 +1634,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
-    <ignoredError sqref="F21 F17" emptyCellReference="1"/>
+    <ignoredError sqref="F17" emptyCellReference="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId1"/>
   <extLst>

</xml_diff>

<commit_message>
even more docs - main writeup of report is finished. need to rewrite first bits
</commit_message>
<xml_diff>
--- a/FYP Finances.xlsx
+++ b/FYP Finances.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ordered Components" sheetId="1" r:id="rId1"/>
+    <sheet name="Cost of 0.2.04" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="60">
   <si>
     <t>Order Code</t>
   </si>
@@ -218,13 +219,29 @@
   </si>
   <si>
     <t>PAID MYSELF</t>
+  </si>
+  <si>
+    <t>Finger Board Components</t>
+  </si>
+  <si>
+    <t>Arduino Shield Components</t>
+  </si>
+  <si>
+    <t>Cost of 1 Board</t>
+  </si>
+  <si>
+    <t>Cost of 3 Boards</t>
+  </si>
+  <si>
+    <t>Cost of 1 Shield</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.000;[Red]\-&quot;£&quot;#,##0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
@@ -314,7 +331,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="143">
+  <cellStyleXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -458,8 +475,48 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -474,8 +531,10 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="143">
+  <cellStyles count="183">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -547,6 +606,26 @@
     <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -618,6 +697,26 @@
     <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -949,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1373,7 +1472,7 @@
         <v>5</v>
       </c>
       <c r="F20" s="1">
-        <f>IF(NOT(ISBLANK($D20)),$D20*$E20,"")</f>
+        <f t="shared" ref="F20:F29" si="1">IF(NOT(ISBLANK($D20)),$D20*$E20,"")</f>
         <v>69.55</v>
       </c>
     </row>
@@ -1394,7 +1493,7 @@
         <v>5</v>
       </c>
       <c r="F21" s="1">
-        <f>IF(NOT(ISBLANK($D21)),$D21*$E21,"")</f>
+        <f t="shared" si="1"/>
         <v>2.8050000000000002</v>
       </c>
     </row>
@@ -1415,7 +1514,7 @@
         <v>5</v>
       </c>
       <c r="F22" s="1">
-        <f>IF(NOT(ISBLANK($D22)),$D22*$E22,"")</f>
+        <f t="shared" si="1"/>
         <v>1.07</v>
       </c>
     </row>
@@ -1436,7 +1535,7 @@
         <v>10</v>
       </c>
       <c r="F23" s="1">
-        <f>IF(NOT(ISBLANK($D23)),$D23*$E23,"")</f>
+        <f t="shared" si="1"/>
         <v>0.15699999999999997</v>
       </c>
     </row>
@@ -1457,7 +1556,7 @@
         <v>10</v>
       </c>
       <c r="F24" s="1">
-        <f>IF(NOT(ISBLANK($D24)),$D24*$E24,"")</f>
+        <f t="shared" si="1"/>
         <v>2.09</v>
       </c>
     </row>
@@ -1478,7 +1577,7 @@
         <v>5</v>
       </c>
       <c r="F25" s="1">
-        <f>IF(NOT(ISBLANK($D25)),$D25*$E25,"")</f>
+        <f t="shared" si="1"/>
         <v>8.8999999999999996E-2</v>
       </c>
     </row>
@@ -1499,7 +1598,7 @@
         <v>5</v>
       </c>
       <c r="F26" s="1">
-        <f>IF(NOT(ISBLANK($D26)),$D26*$E26,"")</f>
+        <f t="shared" si="1"/>
         <v>1.29</v>
       </c>
     </row>
@@ -1520,7 +1619,7 @@
         <v>25</v>
       </c>
       <c r="F27" s="1">
-        <f>IF(NOT(ISBLANK($D27)),$D27*$E27,"")</f>
+        <f t="shared" si="1"/>
         <v>0.91</v>
       </c>
     </row>
@@ -1541,7 +1640,7 @@
         <v>10</v>
       </c>
       <c r="F28" s="1">
-        <f>IF(NOT(ISBLANK($D28)),$D28*$E28,"")</f>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
     </row>
@@ -1562,7 +1661,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="1">
-        <f>IF(NOT(ISBLANK($D29)),$D29*$E29,"")</f>
+        <f t="shared" si="1"/>
         <v>8.51</v>
       </c>
     </row>
@@ -1643,4 +1742,428 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="82.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="82.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="1">
+        <v>11.99</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" ref="F3:F11" si="0">IF(NOT(ISBLANK($D3)),$D3*$E3,"")</f>
+        <v>11.99</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="1">
+        <v>13.79</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3" s="1">
+        <f>IF(NOT(ISBLANK($K3)),$K3*$L3,"")</f>
+        <v>27.58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="1">
+        <v>13.91</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="0"/>
+        <v>13.91</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1368640</v>
+      </c>
+      <c r="J4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="L4">
+        <v>3</v>
+      </c>
+      <c r="M4" s="1">
+        <f t="shared" ref="M4:M12" si="1">IF(NOT(ISBLANK($K4)),$K4*$L4,"")</f>
+        <v>1.6830000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1368640</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.56100000000000005</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="2">
+        <v>3088005</v>
+      </c>
+      <c r="J5" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1.78E-2</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" si="1"/>
+        <v>5.3400000000000003E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3087827</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.5699999999999999E-2</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5699999999999999E-2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="1">
+        <v>3.6400000000000002E-2</v>
+      </c>
+      <c r="L6">
+        <v>3</v>
+      </c>
+      <c r="M6" s="1">
+        <f t="shared" si="1"/>
+        <v>0.10920000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="H7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="1">
+        <v>1.86</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7" s="1">
+        <f t="shared" si="1"/>
+        <v>1.86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3088005</v>
+      </c>
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1.78E-2</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>1.78E-2</v>
+      </c>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="1">
+        <v>3.6400000000000002E-2</v>
+      </c>
+      <c r="E10">
+        <v>7</v>
+      </c>
+      <c r="F10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.25480000000000003</v>
+      </c>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1844418</v>
+      </c>
+      <c r="C11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1502746</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <f>IF(NOT(ISBLANK($D12)),$D12*$E12,"")</f>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="M12" s="1"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="3"/>
+      <c r="D15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="10">
+        <f>SUM($F$3:$F$12)</f>
+        <v>28.565299999999997</v>
+      </c>
+      <c r="L15" s="3"/>
+      <c r="M15" s="11"/>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="11">
+        <f>3*F15</f>
+        <v>85.695899999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="D18" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="10">
+        <f>SUM($M$3:$M$12)</f>
+        <v>31.285599999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="3"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="D20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="11">
+        <f>SUM(F16+F18)</f>
+        <v>116.9815</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>